<commit_message>
added client code in rfc-ssl-vision-client
</commit_message>
<xml_diff>
--- a/hardware/gen5/ControlBoard/control_board_BOM.xlsx
+++ b/hardware/gen5/ControlBoard/control_board_BOM.xlsx
@@ -1,24 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joncr_000\robocup\robocup-ee\hardware\gen5\ControlBoard\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27729"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="24720" windowHeight="13480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ControlModule_BOM" localSheetId="0">Sheet1!$A$1:$E$22</definedName>
+    <definedName name="ControlModule_BOM" localSheetId="0">Sheet1!$A$1:$E$23</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -46,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="98">
   <si>
     <t>Partlist</t>
   </si>
@@ -259,6 +257,78 @@
   </si>
   <si>
     <t>CKN9087CT-ND</t>
+  </si>
+  <si>
+    <t>CT2194MST-ND</t>
+  </si>
+  <si>
+    <t>311-1.0KARCT-ND</t>
+  </si>
+  <si>
+    <t>R2,R5,R8,R9</t>
+  </si>
+  <si>
+    <t>311-0.0ARCT-ND</t>
+  </si>
+  <si>
+    <t>311-10.0CRCT-ND</t>
+  </si>
+  <si>
+    <t>311-100CRCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/8665</t>
+  </si>
+  <si>
+    <t>1276-2450-1-ND</t>
+  </si>
+  <si>
+    <t>1276-1066-1-ND</t>
+  </si>
+  <si>
+    <t>1276-1015-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 478-3051-1-ND</t>
+  </si>
+  <si>
+    <t>478-8410-1-ND</t>
+  </si>
+  <si>
+    <t>BA33BC0FP-E2CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">160-1457-1-ND (red) </t>
+  </si>
+  <si>
+    <t>160-1456-1-ND (green)</t>
+  </si>
+  <si>
+    <t>160-1406-1-ND (yellow)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">754-1156-1-ND (orange) </t>
+  </si>
+  <si>
+    <t>160-1166-1-ND (amber)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 160-1643-1-ND (blue)</t>
+  </si>
+  <si>
+    <t>SEE BELOW</t>
+  </si>
+  <si>
+    <t>We could likely scrap the voltage regulator</t>
+  </si>
+  <si>
+    <t>and send 3.3 from the main board to this board.</t>
+  </si>
+  <si>
+    <t>587-1932-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3M9525-ND </t>
   </si>
   <si>
     <r>
@@ -270,94 +340,21 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>3M9459-ND (male)</t>
+      <t xml:space="preserve">3M9459-ND </t>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> or 3M9525-ND (female)</t>
-    </r>
-  </si>
-  <si>
-    <t>CT2194MST-ND</t>
-  </si>
-  <si>
-    <t>311-1.0KARCT-ND</t>
-  </si>
-  <si>
-    <t>R2,R5,R8,R9</t>
-  </si>
-  <si>
-    <t>311-0.0ARCT-ND</t>
-  </si>
-  <si>
-    <t>311-10.0CRCT-ND</t>
-  </si>
-  <si>
-    <t>311-100CRCT-ND</t>
-  </si>
-  <si>
-    <t>https://www.sparkfun.com/products/8665</t>
-  </si>
-  <si>
-    <t>1276-2450-1-ND</t>
-  </si>
-  <si>
-    <t>1276-1066-1-ND</t>
-  </si>
-  <si>
-    <t>1276-1015-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 478-3051-1-ND</t>
-  </si>
-  <si>
-    <t>478-8410-1-ND</t>
-  </si>
-  <si>
-    <t>BA33BC0FP-E2CT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">160-1457-1-ND (red) </t>
-  </si>
-  <si>
-    <t>160-1456-1-ND (green)</t>
-  </si>
-  <si>
-    <t>160-1406-1-ND (yellow)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">754-1156-1-ND (orange) </t>
-  </si>
-  <si>
-    <t>160-1166-1-ND (amber)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 160-1643-1-ND (blue)</t>
-  </si>
-  <si>
-    <t>SEE BELOW</t>
-  </si>
-  <si>
-    <t>We could likely scrap the voltage regulator</t>
-  </si>
-  <si>
-    <t>and send 3.3 from the main board to this board.</t>
-  </si>
-  <si>
-    <t>587-1932-1-ND</t>
+  </si>
+  <si>
+    <t>PIN HEADER female</t>
+  </si>
+  <si>
+    <t>PIN HEADER male</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -381,6 +378,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -399,16 +404,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -472,7 +487,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -524,7 +539,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -718,7 +733,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -726,23 +741,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="G23" sqref="A4:G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="52.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.44140625" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -759,7 +774,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -782,7 +797,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -796,13 +811,13 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G4">
         <v>0.99</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -819,13 +834,13 @@
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G5">
         <v>0.65</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -842,13 +857,13 @@
         <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G6">
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -865,13 +880,13 @@
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G7">
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -888,13 +903,13 @@
         <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G8">
         <v>0.42</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -911,13 +926,13 @@
         <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G9">
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -931,10 +946,10 @@
         <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -957,7 +972,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -974,15 +989,15 @@
         <v>29</v>
       </c>
       <c r="F12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G12">
         <v>0.1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s">
         <v>30</v>
@@ -997,13 +1012,13 @@
         <v>29</v>
       </c>
       <c r="F13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G13">
         <v>0.1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -1020,13 +1035,13 @@
         <v>29</v>
       </c>
       <c r="F14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G14">
         <v>0.1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -1043,13 +1058,13 @@
         <v>29</v>
       </c>
       <c r="F15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G15">
         <v>0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -1072,7 +1087,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1086,187 +1101,213 @@
         <v>37</v>
       </c>
       <c r="E17" t="s">
+        <v>96</v>
+      </c>
+      <c r="F17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" t="s">
         <v>38</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F19" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" t="s">
         <v>71</v>
       </c>
-      <c r="G17">
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" t="s">
-        <v>43</v>
-      </c>
-      <c r="F19" t="s">
-        <v>72</v>
-      </c>
-      <c r="G19">
+      <c r="G20">
         <v>0.76</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
         <v>44</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>45</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>45</v>
       </c>
-      <c r="D20">
+      <c r="D21">
         <v>805</v>
       </c>
-      <c r="F20" t="s">
-        <v>94</v>
-      </c>
-      <c r="G20">
+      <c r="F21" t="s">
+        <v>93</v>
+      </c>
+      <c r="G21">
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
         <v>46</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>47</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>47</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>48</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E22" t="s">
         <v>49</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F22" t="s">
         <v>57</v>
       </c>
-      <c r="G21">
+      <c r="G22">
         <v>3.58</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
         <v>50</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>51</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>51</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>52</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E23" t="s">
         <v>53</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G22">
+      <c r="F23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G23">
         <v>24.95</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F24" s="1" t="s">
+    <row r="25" spans="1:7">
+      <c r="F25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>92</v>
-      </c>
-      <c r="F25" t="s">
-        <v>85</v>
-      </c>
-      <c r="G25">
-        <v>0.34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7">
       <c r="B26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G26">
         <v>0.34</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7">
+      <c r="B27" t="s">
+        <v>92</v>
+      </c>
       <c r="F27" t="s">
+        <v>85</v>
+      </c>
+      <c r="G27">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="F28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G28">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="F29" t="s">
         <v>87</v>
       </c>
-      <c r="G27">
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F28" t="s">
+      <c r="G29">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="F30" t="s">
         <v>88</v>
       </c>
-      <c r="G28">
-        <v>0.41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F29" t="s">
+      <c r="G30">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="F31" t="s">
         <v>89</v>
       </c>
-      <c r="G29">
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F30" t="s">
-        <v>90</v>
-      </c>
-      <c r="G30">
+      <c r="G31">
         <v>0.39</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F22" r:id="rId1"/>
+    <hyperlink ref="F23" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>